<commit_message>
v1.4.0: Multi-tenant, Excel import improvements, summary AI parsing
Features:
- Multi-tenant organization separation with member management
- System admin panel for organization creation
- Enhanced Excel import with drag & drop, selective import
- AI-powered summary image parsing (Cloud Vision + Claude API)
- New clinical symptoms: thirst, polyuria, vomiting, abdominal pain, etc.
- Bulk delete all patient data button

Technical:
- Added OrganizationContext and OrganizationProvider
- Added processSummaryImage Cloud Function
- Updated Firestore security rules for organizations
- Updated manual.html and README.md

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-data/sample_1型糖尿病慢性期.xlsx
+++ b/sample-data/sample_1型糖尿病慢性期.xlsx
@@ -771,7 +771,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -789,95 +789,73 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2024-06-01</v>
+        <v>2024-06-20</v>
       </c>
       <c r="B2" t="str">
-        <v>診断</v>
+        <v>低血糖</v>
       </c>
       <c r="C2" t="str">
-        <v>8歳女児、DKAで発症した1型糖尿病。抗GAD抗体陽性</v>
+        <v>血糖52mg/dL、冷汗・手指振戦、補食で回復</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2024-06-15</v>
+        <v>2024-07-05</v>
       </c>
       <c r="B3" t="str">
-        <v>退院</v>
+        <v>低血糖</v>
       </c>
       <c r="C3" t="str">
-        <v>インスリン自己注射・血糖自己測定習得し退院</v>
+        <v>血糖48mg/dL、運動後、ブドウ糖摂取</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2024-07-15</v>
+        <v>2024-07-25</v>
       </c>
       <c r="B4" t="str">
-        <v>外来</v>
+        <v>高血糖</v>
       </c>
       <c r="C4" t="str">
-        <v>HbA1c 10.8%、インスリン量調整</v>
+        <v>血糖320mg/dL、インスリン打ち忘れ</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2024-09-01</v>
+        <v>2024-08-10</v>
       </c>
       <c r="B5" t="str">
-        <v>外来</v>
+        <v>低血糖</v>
       </c>
       <c r="C5" t="str">
-        <v>HbA1c 9.2%、学校生活順調。カーボカウント導入</v>
+        <v>血糖55mg/dL、夕食遅延時</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2024-10-15</v>
+        <v>2024-09-15</v>
       </c>
       <c r="B6" t="str">
-        <v>外来</v>
+        <v>低血糖</v>
       </c>
       <c r="C6" t="str">
-        <v>HbA1c 8.5%、低血糖エピソード減少</v>
+        <v>血糖60mg/dL、体育後、軽度</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2024-12-01</v>
+        <v>2024-11-20</v>
       </c>
       <c r="B7" t="str">
-        <v>外来</v>
+        <v>高血糖</v>
       </c>
       <c r="C7" t="str">
-        <v>HbA1c 7.8%、良好なコントロール</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2025-01-15</v>
-      </c>
-      <c r="B8" t="str">
-        <v>外来</v>
-      </c>
-      <c r="C8" t="str">
-        <v>HbA1c 7.4%、目標に近づく</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2025-03-01</v>
-      </c>
-      <c r="B9" t="str">
-        <v>外来</v>
-      </c>
-      <c r="C9" t="str">
-        <v>HbA1c 7.0%達成！学校・運動問題なし</v>
+        <v>血糖280mg/dL、感冒時sick day</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>